<commit_message>
whole map ready + changes in tables
</commit_message>
<xml_diff>
--- a/mapa.xlsx
+++ b/mapa.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDIA\BAZY DANYCH\PROJEKT NA ZALICZENIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C616560-87DE-46B2-BD9E-573414F5CB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFACABB0-03D1-4BA0-B20B-A456D6C18175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DA05E3E6-6C81-40EF-8969-0DDEDB41C0B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>faktura_Numer</t>
   </si>
@@ -109,7 +107,97 @@
     <t>faktura_ID</t>
   </si>
   <si>
-    <t>produkt_Ilość</t>
+    <t>BUTY</t>
+  </si>
+  <si>
+    <t>KASKI</t>
+  </si>
+  <si>
+    <t>KURTKI</t>
+  </si>
+  <si>
+    <t>REKAWICE</t>
+  </si>
+  <si>
+    <t>SPODNIE</t>
+  </si>
+  <si>
+    <t>AKCESORIA</t>
+  </si>
+  <si>
+    <t>PRACOWNICY</t>
+  </si>
+  <si>
+    <t>produkt_Marka</t>
+  </si>
+  <si>
+    <t>produkt_Model</t>
+  </si>
+  <si>
+    <t>produkt_Typ</t>
+  </si>
+  <si>
+    <t>rodzaj_Zapięcia</t>
+  </si>
+  <si>
+    <t>czy_Wodoodporne</t>
+  </si>
+  <si>
+    <t>produkt_Cena</t>
+  </si>
+  <si>
+    <t>produkt_Ilosc</t>
+  </si>
+  <si>
+    <t>produkt_Rozmiar</t>
+  </si>
+  <si>
+    <t>czy_z_Pinlockiem</t>
+  </si>
+  <si>
+    <t>pracownicy_ID</t>
+  </si>
+  <si>
+    <t>pracownik_Imie</t>
+  </si>
+  <si>
+    <t>pracownik_Nazwisko</t>
+  </si>
+  <si>
+    <t>pracownik_Płeć</t>
+  </si>
+  <si>
+    <t>pracownik_Data_Zatrudnienia</t>
+  </si>
+  <si>
+    <t>pracownik_Stanowisko</t>
+  </si>
+  <si>
+    <t>pracownik_pensja</t>
+  </si>
+  <si>
+    <t>klienci_ID</t>
+  </si>
+  <si>
+    <t>SZCZEGÓŁY_ZAMÓWIEŃ</t>
+  </si>
+  <si>
+    <t>zamowienie_Cena</t>
+  </si>
+  <si>
+    <t>czy_Wodoodporna</t>
+  </si>
+  <si>
+    <t>czy_Ocieplana</t>
+  </si>
+  <si>
+    <t>czy_Podgrzewane</t>
+  </si>
+  <si>
+    <t>czy_Ocieplane</t>
+  </si>
+  <si>
+    <t>klient_kod_Pocztowy</t>
   </si>
 </sst>
 </file>
@@ -125,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,13 +228,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,11 +257,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -482,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71A8A9F-E005-4A1B-84EA-83221CBDCAAD}">
-  <dimension ref="C4:G23"/>
+  <dimension ref="C4:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,65 +588,130 @@
     <col min="3" max="3" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.21875" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="11" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
@@ -561,68 +721,227 @@
       <c r="G11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="3" t="s">
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.3">
       <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="3" t="s">
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>